<commit_message>
update corona report excel manually after fix #55
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-01-10.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-01-10.xlsx
@@ -141,10 +141,10 @@
     <t xml:space="preserve">165</t>
   </si>
   <si>
-    <t xml:space="preserve">183</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,9 %</t>
+    <t xml:space="preserve">184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">- Davon 60-bis-79-Jährige</t>
@@ -165,10 +165,10 @@
     <t xml:space="preserve">306</t>
   </si>
   <si>
-    <t xml:space="preserve">333</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,8 %</t>
+    <t xml:space="preserve">334</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,2 %</t>
   </si>
   <si>
     <t xml:space="preserve">Regionen mit 7-TI bei Über-60-Jährigen:</t>
@@ -376,13 +376,13 @@
     <t xml:space="preserve">60 bis 79 Jahre</t>
   </si>
   <si>
-    <t xml:space="preserve">910 ( 4,7%)</t>
+    <t xml:space="preserve">912 ( 4,7%)</t>
   </si>
   <si>
     <t xml:space="preserve">1091 ( 4,6%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 19,9%</t>
+    <t xml:space="preserve"> 19,6%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
@@ -400,13 +400,13 @@
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">3621 ( 2,8%)</t>
+    <t xml:space="preserve">3623 ( 2,8%)</t>
   </si>
   <si>
     <t xml:space="preserve">4461 ( 2,9%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> 23,2%</t>
+    <t xml:space="preserve"> 23,1%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
@@ -1785,7 +1785,7 @@
         <v>173</v>
       </c>
       <c r="D2" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E2" t="n">
         <v>17</v>
@@ -1819,7 +1819,7 @@
         <v>169</v>
       </c>
       <c r="D4" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E4" t="n">
         <v>15</v>
@@ -1887,10 +1887,10 @@
         <v>157</v>
       </c>
       <c r="D8" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E8" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -1904,7 +1904,7 @@
         <v>162</v>
       </c>
       <c r="D9" t="n">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E9" t="n">
         <v>21</v>
@@ -1955,7 +1955,7 @@
         <v>152</v>
       </c>
       <c r="D12" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E12" t="n">
         <v>23</v>
@@ -1989,7 +1989,7 @@
         <v>186</v>
       </c>
       <c r="D14" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E14" t="n">
         <v>33</v>

</xml_diff>